<commit_message>
eddy ni 2000-2001 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni0001/individueel_eindstand_dworp_123_0001.xlsx
+++ b/_data/ni/ni0001/individueel_eindstand_dworp_123_0001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>Matthijs Luc</t>
   </si>
   <si>
-    <t>101 KAOSK 5</t>
-  </si>
-  <si>
     <t>Sunnerberg Constantin</t>
   </si>
   <si>
@@ -358,9 +355,6 @@
     <t>Hoffelinck Jean-Marie junior</t>
   </si>
   <si>
-    <t>472 Mercatel 2</t>
-  </si>
-  <si>
     <t>Vandenbussche Thibaut</t>
   </si>
   <si>
@@ -743,6 +737,12 @@
   </si>
   <si>
     <t>244 WTTC Ukkel 3</t>
+  </si>
+  <si>
+    <t>101 KAOSK Antwerpen 5</t>
+  </si>
+  <si>
+    <t>472 Mercatel Sint-Amandsberg 2</t>
   </si>
 </sst>
 </file>
@@ -1838,7 +1838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2029,7 +2029,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2177,7 +2177,7 @@
         <v>53767</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D8" s="18">
         <v>1660</v>
@@ -2268,7 +2268,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2320,7 +2320,7 @@
         <v>81949</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D15" s="18">
         <v>1946</v>
@@ -2352,7 +2352,7 @@
         <v>67253</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" s="18">
         <v>1915</v>
@@ -2384,7 +2384,7 @@
         <v>81981</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" s="18">
         <v>1906</v>
@@ -2416,7 +2416,7 @@
         <v>78395</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D18" s="18">
         <v>1925</v>
@@ -2475,7 +2475,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2559,7 +2559,7 @@
         <v>48194</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D24" s="18">
         <v>1870</v>
@@ -2591,7 +2591,7 @@
         <v>34126</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D25" s="18">
         <v>1819</v>
@@ -2623,7 +2623,7 @@
         <v>6173</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D26" s="18">
         <v>1516</v>
@@ -2865,7 +2865,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -2925,7 +2925,7 @@
         <v>18686</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J5" s="18">
         <v>2039</v>
@@ -2989,7 +2989,7 @@
         <v>7471</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J7" s="18">
         <v>1768</v>
@@ -3021,7 +3021,7 @@
         <v>58165</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J8" s="18">
         <v>1617</v>
@@ -3104,7 +3104,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -3164,7 +3164,7 @@
         <v>64297</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J15" s="18">
         <v>1923</v>
@@ -3196,7 +3196,7 @@
         <v>82571</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J16" s="18">
         <v>1704</v>
@@ -3228,7 +3228,7 @@
         <v>64092</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J17" s="18">
         <v>1503</v>
@@ -3260,7 +3260,7 @@
         <v>63037</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J18" s="18">
         <v>1363</v>
@@ -3311,7 +3311,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="J21" s="1"/>
       <c r="L21" s="69" t="s">
@@ -3375,7 +3375,7 @@
         <v>25836</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J23" s="18">
         <v>1846</v>
@@ -3407,7 +3407,7 @@
         <v>29122</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J24" s="18">
         <v>1833</v>
@@ -3471,7 +3471,7 @@
         <v>47040</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J26" s="18">
         <v>1763</v>
@@ -3646,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3685,7 +3685,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>100</v>
+        <v>237</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3924,7 +3924,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3976,7 +3976,7 @@
         <v>74349</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="18">
         <v>2078</v>
@@ -4008,7 +4008,7 @@
         <v>65544</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="18">
         <v>1915</v>
@@ -4040,7 +4040,7 @@
         <v>25844</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="18">
         <v>1915</v>
@@ -4072,7 +4072,7 @@
         <v>63886</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="18">
         <v>1763</v>
@@ -4131,7 +4131,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -4183,7 +4183,7 @@
         <v>52060</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="18">
         <v>1882</v>
@@ -4215,7 +4215,7 @@
         <v>80748</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="18">
         <v>1861</v>
@@ -4247,7 +4247,7 @@
         <v>21351</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="18">
         <v>1859</v>
@@ -4279,7 +4279,7 @@
         <v>43893</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="18">
         <v>1329</v>
@@ -4472,7 +4472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ280"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4581,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>37</v>
@@ -4732,7 +4734,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C5" s="41">
         <v>2</v>
@@ -4883,7 +4885,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="41">
         <v>2</v>
@@ -5034,7 +5036,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C7" s="41">
         <v>1.5</v>
@@ -5185,7 +5187,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8" s="41">
         <v>1.5</v>
@@ -5336,7 +5338,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C9" s="41">
         <v>1</v>
@@ -5487,7 +5489,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C10" s="41">
         <v>2.5</v>
@@ -5638,7 +5640,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11" s="41">
         <v>1</v>
@@ -5940,7 +5942,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C13" s="41">
         <v>1</v>
@@ -6091,7 +6093,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C14" s="41">
         <v>0.5</v>
@@ -6242,7 +6244,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>100</v>
+        <v>237</v>
       </c>
       <c r="C15" s="46">
         <v>0.5</v>
@@ -6285,7 +6287,7 @@
         <v>13</v>
       </c>
       <c r="P15" s="49">
-        <f t="shared" ref="P5:P15" si="4">SUM(S15:AD15)</f>
+        <f t="shared" ref="P15" si="4">SUM(S15:AD15)</f>
         <v>2</v>
       </c>
       <c r="Q15" s="49">
@@ -6487,7 +6489,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>37</v>
@@ -6638,7 +6640,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C19" s="41">
         <v>1.5</v>
@@ -6789,7 +6791,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C20" s="41">
         <v>2</v>
@@ -6940,7 +6942,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C21" s="41">
         <v>1.5</v>
@@ -7091,7 +7093,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C22" s="41">
         <v>2</v>
@@ -7242,7 +7244,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C23" s="41">
         <v>1</v>
@@ -7393,7 +7395,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C24" s="41">
         <v>1.5</v>
@@ -7544,7 +7546,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C25" s="41">
         <v>1</v>
@@ -7695,7 +7697,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="41">
         <v>1</v>
@@ -7997,7 +7999,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C28" s="41">
         <v>0</v>
@@ -8148,7 +8150,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C29" s="46">
         <v>2</v>
@@ -8191,7 +8193,7 @@
         <v>15.5</v>
       </c>
       <c r="P29" s="49">
-        <f t="shared" ref="P19:P29" si="20">SUM(S29:AD29)</f>
+        <f t="shared" ref="P29" si="20">SUM(S29:AD29)</f>
         <v>2.5</v>
       </c>
       <c r="Q29" s="49">
@@ -8393,7 +8395,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>37</v>
@@ -8544,7 +8546,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C33" s="41">
         <v>1.5</v>
@@ -8846,7 +8848,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C35" s="41">
         <v>2</v>
@@ -8997,7 +8999,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C36" s="41">
         <v>1.5</v>
@@ -9148,7 +9150,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C37" s="41">
         <v>1</v>
@@ -9299,7 +9301,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C38" s="41">
         <v>1.5</v>
@@ -9450,7 +9452,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C39" s="41">
         <v>1.5</v>
@@ -9601,7 +9603,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C40" s="41">
         <v>0.5</v>
@@ -9752,7 +9754,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="C41" s="41">
         <v>2</v>
@@ -9903,7 +9905,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C42" s="41">
         <v>0.5</v>
@@ -10054,7 +10056,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C43" s="46">
         <v>1</v>
@@ -14998,7 +15000,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15058,7 +15060,7 @@
         <v>25186</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J5" s="18">
         <v>2110</v>
@@ -15154,7 +15156,7 @@
         <v>25917</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J8" s="18">
         <v>1479</v>
@@ -15237,7 +15239,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -15297,7 +15299,7 @@
         <v>87068</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J15" s="18">
         <v>1879</v>
@@ -15329,7 +15331,7 @@
         <v>19933</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J16" s="18">
         <v>1864</v>
@@ -15361,7 +15363,7 @@
         <v>71242</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J17" s="18">
         <v>1726</v>
@@ -15393,7 +15395,7 @@
         <v>90492</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J18" s="18">
         <v>1512</v>
@@ -15434,7 +15436,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -15518,7 +15520,7 @@
         <v>10821</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D24" s="18">
         <v>1958</v>
@@ -15550,7 +15552,7 @@
         <v>32999</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D25" s="18">
         <v>1693</v>
@@ -15582,7 +15584,7 @@
         <v>56782</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D26" s="18">
         <v>1604</v>
@@ -15824,7 +15826,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15884,7 +15886,7 @@
         <v>49778</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J5" s="18">
         <v>1904</v>
@@ -15916,7 +15918,7 @@
         <v>94404</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J6" s="18">
         <v>1930</v>
@@ -15948,7 +15950,7 @@
         <v>56294</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J7" s="18">
         <v>1886</v>
@@ -15980,7 +15982,7 @@
         <v>57789</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J8" s="18">
         <v>1815</v>
@@ -16063,7 +16065,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -16155,7 +16157,7 @@
         <v>67440</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J16" s="18">
         <v>1983</v>
@@ -16187,7 +16189,7 @@
         <v>69311</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J17" s="18">
         <v>1982</v>
@@ -16219,7 +16221,7 @@
         <v>55841</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J18" s="18">
         <v>1400</v>
@@ -16270,7 +16272,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -16640,7 +16642,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -16692,7 +16694,7 @@
         <v>96474</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D5" s="18">
         <v>1878</v>
@@ -16716,7 +16718,7 @@
         <v>1827</v>
       </c>
       <c r="L5" s="68" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M5" s="68"/>
       <c r="N5" s="68"/>
@@ -16729,7 +16731,7 @@
         <v>11037</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" s="18">
         <v>1839</v>
@@ -16761,7 +16763,7 @@
         <v>40746</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D7" s="18">
         <v>1804</v>
@@ -16793,7 +16795,7 @@
         <v>12581</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" s="18">
         <v>1791</v>
@@ -16884,7 +16886,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16936,7 +16938,7 @@
         <v>61948</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D15" s="18">
         <v>1747</v>
@@ -16968,7 +16970,7 @@
         <v>94099</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D16" s="18">
         <v>1732</v>
@@ -17000,7 +17002,7 @@
         <v>90638</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D17" s="18">
         <v>1529</v>
@@ -17032,7 +17034,7 @@
         <v>59951</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D18" s="18">
         <v>1592</v>
@@ -17091,7 +17093,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -17143,7 +17145,7 @@
         <v>876</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D23" s="18">
         <v>2065</v>
@@ -17175,7 +17177,7 @@
         <v>65978</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D24" s="18">
         <v>1971</v>
@@ -17207,7 +17209,7 @@
         <v>46680</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D25" s="18">
         <v>1907</v>
@@ -17481,7 +17483,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -17541,7 +17543,7 @@
         <v>45012</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J5" s="18">
         <v>1824</v>
@@ -17573,7 +17575,7 @@
         <v>44458</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J6" s="18">
         <v>1804</v>
@@ -17720,7 +17722,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -17780,7 +17782,7 @@
         <v>82007</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J15" s="18">
         <v>1831</v>
@@ -17844,7 +17846,7 @@
         <v>396</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J17" s="18">
         <v>1827</v>
@@ -17876,7 +17878,7 @@
         <v>95966</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J18" s="18">
         <v>1708</v>
@@ -17927,7 +17929,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -17987,7 +17989,7 @@
         <v>59811</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J23" s="18">
         <v>1906</v>
@@ -18019,7 +18021,7 @@
         <v>93335</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J24" s="18">
         <v>1841</v>
@@ -18051,7 +18053,7 @@
         <v>89681</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J25" s="18">
         <v>1820</v>
@@ -18083,7 +18085,7 @@
         <v>93360</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J26" s="18">
         <v>1791</v>
@@ -18297,7 +18299,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -18349,7 +18351,7 @@
         <v>2364</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" s="18">
         <v>1872</v>
@@ -18381,7 +18383,7 @@
         <v>24597</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D6" s="18">
         <v>1863</v>
@@ -18413,7 +18415,7 @@
         <v>23281</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D7" s="18">
         <v>1818</v>
@@ -18445,7 +18447,7 @@
         <v>18589</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>79</v>
@@ -18536,7 +18538,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -18588,7 +18590,7 @@
         <v>84735</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D15" s="18">
         <v>1854</v>
@@ -18620,7 +18622,7 @@
         <v>89389</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D16" s="18">
         <v>1707</v>
@@ -18652,7 +18654,7 @@
         <v>79596</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D17" s="18">
         <v>1642</v>
@@ -18684,7 +18686,7 @@
         <v>74161</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D18" s="18">
         <v>1665</v>
@@ -18743,7 +18745,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -18795,7 +18797,7 @@
         <v>38113</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D23" s="18">
         <v>1878</v>
@@ -18827,7 +18829,7 @@
         <v>29467</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D24" s="18">
         <v>1870</v>
@@ -18859,7 +18861,7 @@
         <v>11886</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D25" s="18">
         <v>1842</v>
@@ -18891,7 +18893,7 @@
         <v>45896</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D26" s="18">
         <v>1784</v>
@@ -19133,7 +19135,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -19289,7 +19291,7 @@
         <v>51578</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J8" s="18">
         <v>1620</v>
@@ -19372,7 +19374,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -19432,7 +19434,7 @@
         <v>92916</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J15" s="18">
         <v>1871</v>
@@ -19464,7 +19466,7 @@
         <v>73865</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J16" s="18">
         <v>1676</v>
@@ -19496,7 +19498,7 @@
         <v>78166</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J17" s="18">
         <v>1598</v>
@@ -19528,7 +19530,7 @@
         <v>66621</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>79</v>
@@ -19579,7 +19581,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -19639,7 +19641,7 @@
         <v>4707</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J23" s="18">
         <v>1871</v>
@@ -19703,7 +19705,7 @@
         <v>54500</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J25" s="18">
         <v>1847</v>
@@ -19735,7 +19737,7 @@
         <v>3174</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J26" s="18">
         <v>1791</v>
@@ -19949,7 +19951,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -20001,7 +20003,7 @@
         <v>45632</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D5" s="18">
         <v>1921</v>
@@ -20033,7 +20035,7 @@
         <v>3646</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>79</v>
@@ -20065,7 +20067,7 @@
         <v>3824</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>79</v>
@@ -20097,7 +20099,7 @@
         <v>48062</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D8" s="18">
         <v>1825</v>
@@ -20188,7 +20190,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -20240,7 +20242,7 @@
         <v>72443</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="18">
         <v>1886</v>
@@ -20272,7 +20274,7 @@
         <v>91201</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D16" s="18">
         <v>1861</v>
@@ -20304,7 +20306,7 @@
         <v>60569</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="18">
         <v>1818</v>
@@ -20336,7 +20338,7 @@
         <v>75990</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" s="18">
         <v>1810</v>
@@ -20395,7 +20397,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -20447,7 +20449,7 @@
         <v>36374</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D23" s="18">
         <v>1884</v>
@@ -20479,7 +20481,7 @@
         <v>43311</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D24" s="18">
         <v>1692</v>
@@ -20511,7 +20513,7 @@
         <v>47341</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D25" s="18">
         <v>1783</v>
@@ -20543,7 +20545,7 @@
         <v>43176</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D26" s="18">
         <v>1666</v>
@@ -20785,7 +20787,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -20845,7 +20847,7 @@
         <v>45888</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J5" s="18">
         <v>2053</v>
@@ -20909,7 +20911,7 @@
         <v>26719</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J7" s="18">
         <v>1761</v>
@@ -20941,7 +20943,7 @@
         <v>26808</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J8" s="18">
         <v>1723</v>
@@ -21024,7 +21026,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -21084,7 +21086,7 @@
         <v>85774</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J15" s="18">
         <v>1918</v>
@@ -21116,7 +21118,7 @@
         <v>85472</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J16" s="18">
         <v>1719</v>
@@ -21148,7 +21150,7 @@
         <v>90981</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J17" s="18">
         <v>1642</v>
@@ -21180,7 +21182,7 @@
         <v>66206</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J18" s="18">
         <v>1193</v>
@@ -21231,7 +21233,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -21291,7 +21293,7 @@
         <v>35360</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J23" s="18">
         <v>1839</v>
@@ -21323,7 +21325,7 @@
         <v>23434</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J24" s="18">
         <v>1882</v>
@@ -21355,7 +21357,7 @@
         <v>16021</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J25" s="18">
         <v>1894</v>
@@ -21387,7 +21389,7 @@
         <v>35521</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J26" s="18">
         <v>1742</v>

</xml_diff>